<commit_message>
task3 fatto il codice sui 16 test, parametrizzata la funzione train in task 1,2,3
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,20 +472,118 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4134.252371546751</v>
+        <v>4449.200320822603</v>
       </c>
       <c r="C2" t="n">
-        <v>548.9591212462639</v>
+        <v>388.4662306475441</v>
       </c>
       <c r="D2" t="n">
-        <v>3734.581394128892</v>
+        <v>4060.734090175059</v>
       </c>
       <c r="E2" t="n">
-        <v>3757.692590014332</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4910.483130497027</v>
-      </c>
+        <v>4837.666551470147</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Task 1.2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4449.200320822603</v>
+      </c>
+      <c r="C3" t="n">
+        <v>388.4662306475441</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4060.734090175059</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4837.666551470147</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Task 1.3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5079.337457256514</v>
+      </c>
+      <c r="C4" t="n">
+        <v>571.3560627366455</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5650.693519993159</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4507.981394519868</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Task 2.1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>18290.62894347315</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6147.148928657862</v>
+      </c>
+      <c r="D5" t="n">
+        <v>12143.48001481529</v>
+      </c>
+      <c r="E5" t="n">
+        <v>24437.77787213101</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Task 2.2</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>18290.62894347315</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6147.148928657862</v>
+      </c>
+      <c r="D6" t="n">
+        <v>12143.48001481529</v>
+      </c>
+      <c r="E6" t="n">
+        <v>24437.77787213101</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Task 3.1.1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4192.381535149367</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3017.902992305311</v>
+      </c>
+      <c r="D7" t="n">
+        <v>7210.284527454678</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1174.478542844056</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Comments task 3 and 4
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG23"/>
+  <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1637,100 +1637,100 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.01262806359056558</v>
+        <v>0.01064461902086103</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0007026270012153038</v>
+        <v>0.0005977783134932873</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01220863671141525</v>
+        <v>0.01023751881235292</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01239175305993261</v>
+        <v>0.01069353597888126</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01299401382723213</v>
+        <v>0.01090662505092131</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01282771707641304</v>
+        <v>0.01142638351517632</v>
       </c>
       <c r="H12" t="n">
-        <v>0.01218955822630577</v>
+        <v>0.01042385456887589</v>
       </c>
       <c r="I12" t="n">
-        <v>0.01304217471582856</v>
+        <v>0.01089746446422633</v>
       </c>
       <c r="J12" t="n">
-        <v>0.01413221606090462</v>
+        <v>0.01197185602434062</v>
       </c>
       <c r="K12" t="n">
-        <v>0.01240941044343915</v>
+        <v>0.01040914435577777</v>
       </c>
       <c r="L12" t="n">
-        <v>0.01248858965244989</v>
+        <v>0.01069215975615522</v>
       </c>
       <c r="M12" t="n">
-        <v>0.01170154744888171</v>
+        <v>0.01000714674972099</v>
       </c>
       <c r="N12" t="n">
-        <v>0.01233462510299587</v>
+        <v>0.01015238800555611</v>
       </c>
       <c r="O12" t="n">
-        <v>0.01298815282924202</v>
+        <v>0.01087924733372676</v>
       </c>
       <c r="P12" t="n">
-        <v>0.01173494076117158</v>
+        <v>0.0097993223693</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0121332657970808</v>
+        <v>0.01007686997159644</v>
       </c>
       <c r="R12" t="n">
-        <v>0.01214867564971594</v>
+        <v>0.01018823998682908</v>
       </c>
       <c r="S12" t="n">
-        <v>0.01221581784747909</v>
+        <v>0.0102420787240653</v>
       </c>
       <c r="T12" t="n">
-        <v>0.01237582265653565</v>
+        <v>0.01042064613234451</v>
       </c>
       <c r="U12" t="n">
-        <v>0.01248049465646529</v>
+        <v>0.01061791013628076</v>
       </c>
       <c r="V12" t="n">
-        <v>0.01220773034250626</v>
+        <v>0.01031125561989872</v>
       </c>
       <c r="W12" t="n">
-        <v>0.01199609248268396</v>
+        <v>0.0101727840990696</v>
       </c>
       <c r="X12" t="n">
-        <v>0.01297301721610003</v>
+        <v>0.01058454807166361</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.01264603589933758</v>
+        <v>0.01065592379424043</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.01389140310689247</v>
+        <v>0.01169337690567628</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.01480268077767647</v>
+        <v>0.01246221382894587</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.01211953118632274</v>
+        <v>0.01024881006312314</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.01238356261688167</v>
+        <v>0.01042735895887869</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.01303837282164264</v>
+        <v>0.01086263077957389</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.01195923005139547</v>
+        <v>0.009964249901595657</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.01235836851592041</v>
+        <v>0.01070290221748107</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.01366847017611865</v>
+        <v>0.01121012444955634</v>
       </c>
     </row>
     <row r="13">
@@ -2864,6 +2864,109 @@
       </c>
       <c r="AG23" t="n">
         <v>0.01106407795979203</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Task 4</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.01255425673669903</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0006583993878467496</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.01228864237644526</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.01239493831392954</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.01320084748559273</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.0135264380862166</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.01178920175774237</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.01205237801417426</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.0138306402513558</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.01230702130655395</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.0119169713591391</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.0126006423659272</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.01220005656477842</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.0123339049428252</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.01224519318585674</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.01175575738206552</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.0127559384810645</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0.0132778541071266</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.01203126105397126</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0.0121738441414118</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0.01186061735295003</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0.0135572255948135</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0.01261200975557703</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0.01213630682630265</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0.01201770924054356</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>0.01269238361796149</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0.0121447554838243</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>0.01258021438784777</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>0.01309439147371852</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>0.01190520251928036</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>0.01449880473366081</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>0.01284654993831405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run 4 & 5
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -2869,104 +2869,104 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Task 4</t>
+          <t>Task 5.2</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.01056809025693879</v>
+        <v>0.01063110686486934</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0004251419247380778</v>
+        <v>0.0006593205747873491</v>
       </c>
       <c r="D24" t="n">
-        <v>0.01037159892807455</v>
+        <v>0.01043710554316247</v>
       </c>
       <c r="E24" t="n">
-        <v>0.01053392145062811</v>
+        <v>0.01037725881995812</v>
       </c>
       <c r="F24" t="n">
-        <v>0.01074960940189098</v>
+        <v>0.01071944822600781</v>
       </c>
       <c r="G24" t="n">
-        <v>0.01021502555306767</v>
+        <v>0.01127196178817419</v>
       </c>
       <c r="H24" t="n">
-        <v>0.01096049719876997</v>
+        <v>0.01027269198404056</v>
       </c>
       <c r="I24" t="n">
-        <v>0.01024017969239922</v>
+        <v>0.01084408167559385</v>
       </c>
       <c r="J24" t="n">
-        <v>0.01019598347694009</v>
+        <v>0.01086165834018276</v>
       </c>
       <c r="K24" t="n">
-        <v>0.01033018247194936</v>
+        <v>0.009937403691591649</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0104702606927747</v>
+        <v>0.009945927533684838</v>
       </c>
       <c r="M24" t="n">
-        <v>0.01066761632963951</v>
+        <v>0.0100262569883421</v>
       </c>
       <c r="N24" t="n">
-        <v>0.01154692538081481</v>
+        <v>0.01157106240780273</v>
       </c>
       <c r="O24" t="n">
-        <v>0.01082319999272506</v>
+        <v>0.01180676729131343</v>
       </c>
       <c r="P24" t="n">
-        <v>0.01044953265560866</v>
+        <v>0.009879806617262255</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.01053661446667713</v>
+        <v>0.01028222543972634</v>
       </c>
       <c r="R24" t="n">
-        <v>0.0100905247265575</v>
+        <v>0.01016269812056746</v>
       </c>
       <c r="S24" t="n">
-        <v>0.0106131793606767</v>
+        <v>0.01029817565819954</v>
       </c>
       <c r="T24" t="n">
-        <v>0.01044342437098189</v>
+        <v>0.01056886045503612</v>
       </c>
       <c r="U24" t="n">
-        <v>0.01063048843413842</v>
+        <v>0.0105073514402727</v>
       </c>
       <c r="V24" t="n">
-        <v>0.0113227011416644</v>
+        <v>0.01165383831277412</v>
       </c>
       <c r="W24" t="n">
-        <v>0.009883011275346854</v>
+        <v>0.01002025273752969</v>
       </c>
       <c r="X24" t="n">
-        <v>0.01141639539737497</v>
+        <v>0.01108181075739776</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.01015933367157239</v>
+        <v>0.009750670392637361</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.01037784229561048</v>
+        <v>0.01013701511806955</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.01007344352089658</v>
+        <v>0.009871627184213881</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.01074051943846135</v>
+        <v>0.0116820261470679</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.01141365896665312</v>
+        <v>0.01079419456860513</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.01034929149376649</v>
+        <v>0.01030819466498653</v>
       </c>
       <c r="AE24" t="n">
-        <v>0.01078732068471963</v>
+        <v>0.01233586970705188</v>
       </c>
       <c r="AF24" t="n">
-        <v>0.01071003869035931</v>
+        <v>0.01113817766392169</v>
       </c>
       <c r="AG24" t="n">
-        <v>0.009940386547423734</v>
+        <v>0.01038878667090573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update of task 4 and 5
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG27"/>
+  <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2869,7 +2869,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Task 4</t>
+          <t>Task 4.1</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -2972,310 +2972,413 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Task 5.1</t>
+          <t>Task 4.2</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.01061860054157</v>
+        <v>0.01057013667475462</v>
       </c>
       <c r="C25" t="n">
-        <v>0.000642580286161867</v>
+        <v>0.0005005659407863555</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01011433602771769</v>
+        <v>0.01030731884798878</v>
       </c>
       <c r="E25" t="n">
-        <v>0.01027878664917922</v>
+        <v>0.01046173435880525</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0112247207328965</v>
+        <v>0.01103629893751503</v>
       </c>
       <c r="G25" t="n">
-        <v>0.01097195567738501</v>
+        <v>0.01008439654807944</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01046086097790481</v>
+        <v>0.01093962419329085</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0107349103187676</v>
+        <v>0.01015618973961673</v>
       </c>
       <c r="J25" t="n">
-        <v>0.01112181879739266</v>
+        <v>0.0100724451293896</v>
       </c>
       <c r="K25" t="n">
-        <v>0.00991036422911821</v>
+        <v>0.01061491848467104</v>
       </c>
       <c r="L25" t="n">
-        <v>0.009791106984577552</v>
+        <v>0.01033790987375893</v>
       </c>
       <c r="M25" t="n">
-        <v>0.009936914360008499</v>
+        <v>0.01048788691785228</v>
       </c>
       <c r="N25" t="n">
-        <v>0.01162469668166206</v>
+        <v>0.01143696616118029</v>
       </c>
       <c r="O25" t="n">
-        <v>0.01132966042922809</v>
+        <v>0.01092643645155179</v>
       </c>
       <c r="P25" t="n">
-        <v>0.009797751633263232</v>
+        <v>0.01025622278850475</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.0103401854975243</v>
+        <v>0.01073533645900154</v>
       </c>
       <c r="R25" t="n">
-        <v>0.01036179053011395</v>
+        <v>0.01007063401650483</v>
       </c>
       <c r="S25" t="n">
-        <v>0.01030852162287169</v>
+        <v>0.01082403369716303</v>
       </c>
       <c r="T25" t="n">
-        <v>0.01057698299479672</v>
+        <v>0.01050390026902077</v>
       </c>
       <c r="U25" t="n">
-        <v>0.01164732622492706</v>
+        <v>0.01077713568897991</v>
       </c>
       <c r="V25" t="n">
-        <v>0.01163268293930642</v>
+        <v>0.01156918574693464</v>
       </c>
       <c r="W25" t="n">
-        <v>0.009841470971278975</v>
+        <v>0.009712423806234684</v>
       </c>
       <c r="X25" t="n">
-        <v>0.0110799030614077</v>
+        <v>0.01169137996563375</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.009851507301561171</v>
+        <v>0.01008737208311145</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.01065650096284967</v>
+        <v>0.01038533426990044</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.0100474359387504</v>
+        <v>0.01002207990846811</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.0112716359893262</v>
+        <v>0.010892256726454</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.01069247563562356</v>
+        <v>0.01135329705292846</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.009865071640241465</v>
+        <v>0.01023900159137059</v>
       </c>
       <c r="AE25" t="n">
-        <v>0.01204921110082998</v>
+        <v>0.01082215320353932</v>
       </c>
       <c r="AF25" t="n">
-        <v>0.01088192560802101</v>
+        <v>0.01046445840502846</v>
       </c>
       <c r="AG25" t="n">
-        <v>0.01015550472856856</v>
+        <v>0.009835768920159778</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Task 5.2</t>
+          <t>Task 5.1</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.01063110686486934</v>
+        <v>0.01094645632520933</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0006593205747873491</v>
+        <v>0.0009015060449485058</v>
       </c>
       <c r="D26" t="n">
-        <v>0.01043710554316247</v>
+        <v>0.0105947442228127</v>
       </c>
       <c r="E26" t="n">
-        <v>0.01037725881995812</v>
+        <v>0.01064116525558864</v>
       </c>
       <c r="F26" t="n">
-        <v>0.01071944822600781</v>
+        <v>0.01290009441114279</v>
       </c>
       <c r="G26" t="n">
-        <v>0.01127196178817419</v>
+        <v>0.01041402377965366</v>
       </c>
       <c r="H26" t="n">
-        <v>0.01027269198404056</v>
+        <v>0.01052461469724162</v>
       </c>
       <c r="I26" t="n">
-        <v>0.01084408167559385</v>
+        <v>0.01102616963801676</v>
       </c>
       <c r="J26" t="n">
-        <v>0.01086165834018276</v>
+        <v>0.01043513092124959</v>
       </c>
       <c r="K26" t="n">
-        <v>0.009937403691591649</v>
+        <v>0.01007429458308798</v>
       </c>
       <c r="L26" t="n">
-        <v>0.009945927533684838</v>
+        <v>0.01052191798454783</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0100262569883421</v>
+        <v>0.01038607140137711</v>
       </c>
       <c r="N26" t="n">
-        <v>0.01157106240780273</v>
+        <v>0.01169278225280685</v>
       </c>
       <c r="O26" t="n">
-        <v>0.01180676729131343</v>
+        <v>0.01121431387448157</v>
       </c>
       <c r="P26" t="n">
-        <v>0.009879806617262255</v>
+        <v>0.01013278970275092</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.01028222543972634</v>
+        <v>0.01054587546034712</v>
       </c>
       <c r="R26" t="n">
-        <v>0.01016269812056746</v>
+        <v>0.009789165836331638</v>
       </c>
       <c r="S26" t="n">
-        <v>0.01029817565819954</v>
+        <v>0.01057606753487713</v>
       </c>
       <c r="T26" t="n">
-        <v>0.01056886045503612</v>
+        <v>0.01060314049240994</v>
       </c>
       <c r="U26" t="n">
-        <v>0.0105073514402727</v>
+        <v>0.01088286083218916</v>
       </c>
       <c r="V26" t="n">
-        <v>0.01165383831277412</v>
+        <v>0.01169587789401826</v>
       </c>
       <c r="W26" t="n">
-        <v>0.01002025273752969</v>
+        <v>0.01036945468160288</v>
       </c>
       <c r="X26" t="n">
-        <v>0.01108181075739776</v>
+        <v>0.01229077041653039</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.009750670392637361</v>
+        <v>0.01038786501902274</v>
       </c>
       <c r="Z26" t="n">
-        <v>0.01013701511806955</v>
+        <v>0.01114223586665325</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.009871627184213881</v>
+        <v>0.01080742570073047</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.0116820261470679</v>
+        <v>0.0131134659350269</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.01079419456860513</v>
+        <v>0.01209163466560852</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.01030819466498653</v>
+        <v>0.009911310621027784</v>
       </c>
       <c r="AE26" t="n">
-        <v>0.01233586970705188</v>
+        <v>0.01292687250175204</v>
       </c>
       <c r="AF26" t="n">
-        <v>0.01113817766392169</v>
+        <v>0.01086647707732529</v>
       </c>
       <c r="AG26" t="n">
-        <v>0.01038878667090573</v>
+        <v>0.009835076496068487</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>Task 5.2</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.01105812470007133</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.000801530499824401</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.01040134141374233</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.01054155830563586</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.01199250720794866</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.01017678899381777</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.01132816402016193</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.01194004847267183</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.01060357283730544</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.01131292985119929</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.01089105513727888</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.01026045188892836</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.01141995560590436</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.01168005161730688</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.010527887523696</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.01036495060336992</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.009999550651592373</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0.01054947398991609</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.01089902656314451</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0.01152356853482261</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0.01190753122639767</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.01074064948256935</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0.012598873125015</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0.01076845084808825</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0.01174774694955943</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>0.01032694570052849</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>0.01168678052568842</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>0.01152006667137058</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>0.009958183749771426</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>0.01325483482330768</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>0.01089260112675032</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>0.009928193554650223</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>Task 5.3</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>0.01060339761578878</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0.000663766388823935</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0.01016423419856203</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.01031958376122531</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.01159343305243781</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.01120468138345878</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0.01062533396269232</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0.01051067999179003</v>
-      </c>
-      <c r="J27" t="n">
-        <v>0.01150509262491319</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0.009995110985058609</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0.009824227513908964</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0.009870882660994453</v>
-      </c>
-      <c r="N27" t="n">
-        <v>0.01144004940400946</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0.01131116957844972</v>
-      </c>
-      <c r="P27" t="n">
-        <v>0.009846890525716622</v>
-      </c>
-      <c r="Q27" t="n">
-        <v>0.01024172202379465</v>
-      </c>
-      <c r="R27" t="n">
-        <v>0.01026878740394908</v>
-      </c>
-      <c r="S27" t="n">
-        <v>0.01022124778320007</v>
-      </c>
-      <c r="T27" t="n">
-        <v>0.0105273486343247</v>
-      </c>
-      <c r="U27" t="n">
-        <v>0.01050133607886856</v>
-      </c>
-      <c r="V27" t="n">
-        <v>0.01159423947716496</v>
-      </c>
-      <c r="W27" t="n">
-        <v>0.009962261757706294</v>
-      </c>
-      <c r="X27" t="n">
-        <v>0.01126374760757759</v>
-      </c>
-      <c r="Y27" t="n">
-        <v>0.009803952808169005</v>
-      </c>
-      <c r="Z27" t="n">
-        <v>0.01005872218421709</v>
-      </c>
-      <c r="AA27" t="n">
-        <v>0.01016278482474796</v>
-      </c>
-      <c r="AB27" t="n">
-        <v>0.01083290441772231</v>
-      </c>
-      <c r="AC27" t="n">
-        <v>0.01093416867400333</v>
-      </c>
-      <c r="AD27" t="n">
-        <v>0.009970348338668332</v>
-      </c>
-      <c r="AE27" t="n">
-        <v>0.01223222571418951</v>
-      </c>
-      <c r="AF27" t="n">
-        <v>0.01133111101488586</v>
-      </c>
-      <c r="AG27" t="n">
-        <v>0.00998365008725677</v>
+      <c r="B28" t="n">
+        <v>0.01092233396509257</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0008218368162363563</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.01069095317834767</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.01046998944436819</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.01298152631821786</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.01037306942016312</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.0103084622219599</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.01100685503390813</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.01102118488917939</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.01112867270852016</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.01061221438384759</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.01046101830713468</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.01143602718992988</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.01110305415961764</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.01033951649990365</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.01050756696355912</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.009873911427863166</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0.01042816544272811</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.01096483406365935</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0.01067821760227414</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0.01258196408800248</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0.01070875778470997</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0.01247479091767482</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0.01055939637759182</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0.01082003997454337</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>0.009938394700583848</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0.01265017724044342</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0.01082929094785161</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0.009938750174112372</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>0.01205727783434322</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>0.01075549715273997</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>0.009970442504998421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>